<commit_message>
ckt branch new length makeup param
</commit_message>
<xml_diff>
--- a/AE pyTools.extension/AE pyTools.Tab/Electrical.panel/Circuits1.stack/Circuit Tools.pulldown/Load Electrical Parameters.pushbutton/Content/ELEC SHARED PARAM TABLE.xlsx
+++ b/AE pyTools.extension/AE pyTools.Tab/Electrical.panel/Circuits1.stack/Circuit Tools.pulldown/Load Electrical Parameters.pushbutton/Content/ELEC SHARED PARAM TABLE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aevelina\CED_Extensions\AE pyTools.extension\AE pyTools.Tab\Miscellaneous.panel\MiscTools.pulldown\Load Electrical Parameters.pushbutton\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aevelina\CED_Extensions\AE pyTools.extension\AE pyTools.Tab\Electrical.panel\Circuits1.stack\Circuit Tools.pulldown\Load Electrical Parameters.pushbutton\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B83292-DD96-47E0-B5AE-06B0B3705710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{917F13C7-3E2E-493C-891B-48AE8A52ADA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8085" yWindow="1695" windowWidth="30645" windowHeight="17820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32115" yWindow="5400" windowWidth="17355" windowHeight="15480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameter List" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="484">
   <si>
     <t>GUID</t>
   </si>
@@ -1493,6 +1493,12 @@
   </si>
   <si>
     <t>Wire Size_CEDT</t>
+  </si>
+  <si>
+    <t>4d467bf2-9dc1-4086-9279-727c85716211</t>
+  </si>
+  <si>
+    <t>CKT_Length Makeup_CED</t>
   </si>
 </sst>
 </file>
@@ -1891,10 +1897,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B34"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="66" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2896,6 +2902,35 @@
         <v>35</v>
       </c>
     </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="B35" s="7">
+        <v>34</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:H1" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H38">
@@ -2903,22 +2938,22 @@
     </sortState>
   </autoFilter>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="The inserted value is not valid. Please select a value from the dropdown list" sqref="F2:F34" xr:uid="{06D99139-2FA3-4AFB-B1C3-3BEE2A9AAD12}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="The inserted value is not valid. Please select a value from the dropdown list" sqref="F2:F35" xr:uid="{06D99139-2FA3-4AFB-B1C3-3BEE2A9AAD12}">
       <formula1>ParamValues6</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="The inserted value is not valid. Please select a value from the dropdown list" sqref="G2:G34" xr:uid="{1151C22F-EEEC-41FC-9B99-4E6AF0576CD2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="The inserted value is not valid. Please select a value from the dropdown list" sqref="G2:G35" xr:uid="{1151C22F-EEEC-41FC-9B99-4E6AF0576CD2}">
       <formula1>ParamValues7</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="The inserted value is not valid. Please select a value from the dropdown list" sqref="H2:H34" xr:uid="{616A26CB-D9F9-4D1C-BA1B-E708E2CBE0E9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="The inserted value is not valid. Please select a value from the dropdown list" sqref="H2:H35" xr:uid="{616A26CB-D9F9-4D1C-BA1B-E708E2CBE0E9}">
       <formula1>ParamValues8</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="The inserted value is not valid. Please select a value from the dropdown list" sqref="I2:I34" xr:uid="{B1E7E558-C3C7-40E8-8539-FFB9D8F8545E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="The inserted value is not valid. Please select a value from the dropdown list" sqref="I2:I35" xr:uid="{B1E7E558-C3C7-40E8-8539-FFB9D8F8545E}">
       <formula1>ParamValues13</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="The inserted value is not valid. Please select a value from the dropdown list" sqref="D2:D34" xr:uid="{827EEA15-0EC2-40C8-B587-AD980D20E9D0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="The inserted value is not valid. Please select a value from the dropdown list" sqref="D2:D35" xr:uid="{827EEA15-0EC2-40C8-B587-AD980D20E9D0}">
       <formula1>ParamValues4</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="The inserted value is not valid. Please select a value from the dropdown list" sqref="E2:E34" xr:uid="{4E58A52C-D07C-4F2B-B4F2-F5CE0A750771}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="The inserted value is not valid. Please select a value from the dropdown list" sqref="E2:E35" xr:uid="{4E58A52C-D07C-4F2B-B4F2-F5CE0A750771}">
       <formula1>INDIRECT(D2)</formula1>
     </dataValidation>
   </dataValidations>
@@ -5021,15 +5056,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="d3d766bc-3a2e-4b05-abf0-3bfac4a5263f" xsi:nil="true"/>
@@ -5038,6 +5064,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5060,14 +5095,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0ADC3DD0-5BD5-40CE-B970-48D4CA313F4F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F0BD034-2603-47A7-897F-4421320EF50F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -5076,4 +5103,12 @@
     <ds:schemaRef ds:uri="1ce2a17a-c0eb-4821-a205-2297eefe49d7"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0ADC3DD0-5BD5-40CE-B970-48D4CA313F4F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>